<commit_message>
Made the code a lot more modular
</commit_message>
<xml_diff>
--- a/IPtoASN/ip_list.xlsx
+++ b/IPtoASN/ip_list.xlsx
@@ -16,7 +16,8 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
-    <t>178.137.87.242</t>
+    <t xml:space="preserve">178.137.87.242
+</t>
   </si>
   <si>
     <t>Ukraine</t>
@@ -28,7 +29,8 @@
     <t>15895: Kyivstar PJSC</t>
   </si>
   <si>
-    <t>46.148.22.18</t>
+    <t xml:space="preserve">46.148.22.18
+</t>
   </si>
   <si>
     <t>Kharkiv</t>
@@ -37,7 +39,8 @@
     <t>50297: Infium, UAB</t>
   </si>
   <si>
-    <t>201.18.18.173</t>
+    <t xml:space="preserve">201.18.18.173
+</t>
   </si>
   <si>
     <t>Brazil</t>
@@ -46,10 +49,12 @@
     <t>7738: Telemar Norte Leste S.A.</t>
   </si>
   <si>
-    <t>46.148.18.162</t>
-  </si>
-  <si>
-    <t>37.187.129.166</t>
+    <t xml:space="preserve">46.148.18.162
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.187.129.166
+</t>
   </si>
   <si>
     <t>France</t>

</xml_diff>